<commit_message>
Update subtype value define: type/subtype value define set into each packet config file, instead of config basic file
</commit_message>
<xml_diff>
--- a/doc/diagram.xlsx
+++ b/doc/diagram.xlsx
@@ -9,8 +9,37 @@
   <sheets>
     <sheet name="diagram" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>In config.ini, define enable flag</t>
+  </si>
+  <si>
+    <t>Flow of adding new packet type</t>
+  </si>
+  <si>
+    <t>Create /my_sniff/subtype/packet_type folder, and in this folder, create packet_type.py file which includes all fields and value define</t>
+  </si>
+  <si>
+    <t>In  /my_config/config_basic.py,  add func to get enable flag</t>
+  </si>
+  <si>
+    <t>In /packet_config/ folder, create config_xxx.ini (xxx is the packet type name), and update related fields. In /my_config/ folder, add config_xxx.py to get values from ini file</t>
+  </si>
+  <si>
+    <t>in my_flow.py, import config_xxx.py file</t>
+  </si>
+  <si>
+    <t>in my_flow.py, import packet_type.py file</t>
+  </si>
+  <si>
+    <t>update my_flow.py to add this packet type check section</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -85,8 +114,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3115395" y="1143000"/>
-          <a:ext cx="15254248" cy="5266764"/>
+          <a:off x="3084470" y="1143000"/>
+          <a:ext cx="15099621" cy="5266764"/>
           <a:chOff x="6051176" y="2274794"/>
           <a:chExt cx="15074154" cy="5266764"/>
         </a:xfrm>
@@ -1814,8 +1843,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20727440" y="12899571"/>
-          <a:ext cx="3700823" cy="2743200"/>
+          <a:off x="20523333" y="12899571"/>
+          <a:ext cx="3663712" cy="2743200"/>
           <a:chOff x="15945970" y="6745941"/>
           <a:chExt cx="3657600" cy="2743200"/>
         </a:xfrm>
@@ -2008,8 +2037,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20727440" y="6667500"/>
-          <a:ext cx="6452028" cy="2743200"/>
+          <a:off x="20523333" y="6667500"/>
+          <a:ext cx="6383992" cy="2743200"/>
           <a:chOff x="16053546" y="10529048"/>
           <a:chExt cx="6400800" cy="2743200"/>
         </a:xfrm>
@@ -2321,8 +2350,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20727440" y="9775371"/>
-          <a:ext cx="13562560" cy="2743200"/>
+          <a:off x="20523333" y="9775371"/>
+          <a:ext cx="13420303" cy="2743200"/>
           <a:chOff x="19451410" y="9829800"/>
           <a:chExt cx="13719042" cy="2743200"/>
         </a:xfrm>
@@ -3159,8 +3188,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20727440" y="15947571"/>
-          <a:ext cx="3705306" cy="2743200"/>
+          <a:off x="20523333" y="15947571"/>
+          <a:ext cx="3668195" cy="2743200"/>
           <a:chOff x="15945970" y="6745941"/>
           <a:chExt cx="3657600" cy="2743200"/>
         </a:xfrm>
@@ -4074,8 +4103,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3084476" y="13781834"/>
-          <a:ext cx="6462295" cy="2743200"/>
+          <a:off x="3053551" y="13781834"/>
+          <a:ext cx="6400444" cy="2743200"/>
           <a:chOff x="16053546" y="10529048"/>
           <a:chExt cx="6400800" cy="2743200"/>
         </a:xfrm>
@@ -4484,8 +4513,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3061607" y="17311267"/>
-          <a:ext cx="9797143" cy="4953000"/>
+          <a:off x="3030682" y="17311267"/>
+          <a:ext cx="9698182" cy="4953000"/>
           <a:chOff x="3048000" y="17526000"/>
           <a:chExt cx="9753600" cy="4953000"/>
         </a:xfrm>
@@ -5351,8 +5380,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3198776" y="23050500"/>
-          <a:ext cx="11528316" cy="2743200"/>
+          <a:off x="3167851" y="23050500"/>
+          <a:ext cx="11410800" cy="2743200"/>
           <a:chOff x="3198776" y="23186571"/>
           <a:chExt cx="11528316" cy="2743200"/>
         </a:xfrm>
@@ -6482,7 +6511,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>my_logging.py</a:t>
+            <a:t>ctrl</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6497,7 +6526,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>-------------------------------------------------------Logging related</a:t>
+            <a:t>---------------------------------------------------</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6512,8 +6541,56 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>-------------------------------------------------------</a:t>
+            <a:t>Control</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> packet</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------------------------------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -6586,7 +6663,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>my_matplotlib.py</a:t>
+            <a:t>data</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6601,7 +6678,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>-------------------------------------------------------</a:t>
+            <a:t>---------------------------------------------------</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6616,8 +6693,29 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Matplotlib related</a:t>
+            <a:t>Data</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> packet</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr marL="0" indent="0" algn="l"/>
@@ -6631,8 +6729,20 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>-------------------------------------------------------</a:t>
+            <a:t>---------------------------------------------------</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr marL="0" indent="0" algn="l"/>
@@ -6717,7 +6827,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>my_time.py</a:t>
+            <a:t>mgt</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6732,7 +6842,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>-------------------------------------------------------Time stamp related</a:t>
+            <a:t>---------------------------------------------------</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6747,11 +6857,350 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>-------------------------------------------------------</a:t>
+            <a:t>Managetment packet</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------------------------------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>92777</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>105146</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>415407</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>181346</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="87" name="Group 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82397408-32F4-4802-A00A-6B1BDC186671}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="16458459" y="28680146"/>
+          <a:ext cx="6383993" cy="2743200"/>
+          <a:chOff x="16053546" y="10529048"/>
+          <a:chExt cx="6400800" cy="2743200"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="88" name="Rounded Rectangle 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6FD956E-79DE-4405-B227-6F5F556C7144}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16053546" y="10529048"/>
+            <a:ext cx="6400800" cy="2743200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>ctrl/data/mgt</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="90" name="Rounded Rectangle 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9EBBF28-B6BF-40C4-A699-A6CD75B9F4BD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16340416" y="10954871"/>
+            <a:ext cx="2743200" cy="1828800"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent5">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>packet_type.py</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>-------------------------------------------------------</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>-------------------------------------------------------</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="91" name="Rounded Rectangle 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C80A5698-7EF8-48F1-BCB7-CC7C8B93FDBB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19370486" y="10954871"/>
+            <a:ext cx="2743200" cy="1828800"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent5">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>layer_name.py</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>-------------------------------------------------------</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>-------------------------------------------------------</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -7044,14 +7493,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="F167:G174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D132" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N170" sqref="N170"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AG23" sqref="AG23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="167" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F167" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="G168" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F169">
+        <v>0.1</v>
+      </c>
+      <c r="G169" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F170">
+        <v>1</v>
+      </c>
+      <c r="G170" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F171">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G171" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F172">
+        <v>2</v>
+      </c>
+      <c r="G172" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F173">
+        <v>2.1</v>
+      </c>
+      <c r="G173" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F174">
+        <v>3</v>
+      </c>
+      <c r="G174" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>